<commit_message>
date time issue fix
Former-commit-id: 79ff2dfa1b6545f0ee7c32821404e7e2aed8ccf5
</commit_message>
<xml_diff>
--- a/excel_templates/expense-template.xlsx
+++ b/excel_templates/expense-template.xlsx
@@ -49,8 +49,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="166" formatCode="d/mm/yyyy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -102,7 +103,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -114,6 +115,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -399,7 +403,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,150 +441,150 @@
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="G2" s="5"/>
       <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
       <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="G3" s="5"/>
       <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="G4" s="5"/>
       <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="G5" s="5"/>
       <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="G6" s="5"/>
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
       <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="G7" s="5"/>
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="G8" s="5"/>
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="G9" s="5"/>
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="G10" s="5"/>
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="G11" s="5"/>
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="G12" s="5"/>
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
       <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+      <c r="G13" s="5"/>
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="G14" s="5"/>
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="G15" s="5"/>
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="G16" s="5"/>
       <c r="H16" s="4"/>
     </row>
   </sheetData>

</xml_diff>